<commit_message>
agregar cambios de dependencia de xlsx a exceljs
</commit_message>
<xml_diff>
--- a/data/DataDriven.xlsx
+++ b/data/DataDriven.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\arquetipo_pruebas_api_automation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67256DC1-FD33-4AC7-967B-DAC0F5EFA9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F1A72B-E6F5-44FC-954A-3DBBB1244330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{4CEB8AB6-E7B5-4B0E-B37E-4FFA86E7928B}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>0958951059</t>
   </si>
   <si>
-    <t>tetsemai@gmail.com'</t>
-  </si>
-  <si>
     <t>id_category</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>value2test</t>
+  </si>
+  <si>
+    <t>testlast@etst.com</t>
   </si>
 </sst>
 </file>
@@ -198,7 +198,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -537,13 +537,14 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -574,7 +575,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>4444555</v>
+        <v>66665555</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -586,7 +587,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>11</v>
@@ -600,7 +601,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="tetsemai@gmail.com" xr:uid="{23FA6AF4-9344-4210-9730-E5E00A5C531A}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{C17F9A1F-BF9C-4F50-83ED-FED54E47350E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -611,7 +612,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,22 +626,22 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -648,22 +649,22 @@
         <v>401</v>
       </c>
       <c r="B2" s="1">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1">
+        <v>403</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -675,26 +676,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE12C29-7C97-4F22-AD61-0320B3A8733D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>